<commit_message>
Revisi Report (Bissmillah bnr), add Notification Import, Revisi Import
</commit_message>
<xml_diff>
--- a/public/files/template_import_mdc.xlsx
+++ b/public/files/template_import_mdc.xlsx
@@ -8,14 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\HCIS-Cash-Advance\public\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE12972-3787-4ADD-AB90-3013B91F90F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB2A90F-E35E-421A-BE57-91D2B40ED22A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mdc_transactions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -34,9 +45,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>EmployeeID</t>
-  </si>
-  <si>
     <t>No Invoice</t>
   </si>
   <si>
@@ -61,9 +69,6 @@
     <t>Medical Type</t>
   </si>
   <si>
-    <t>Balance</t>
-  </si>
-  <si>
     <t>Balance Verif</t>
   </si>
   <si>
@@ -80,13 +85,19 @@
   </si>
   <si>
     <t>Detail Template</t>
+  </si>
+  <si>
+    <t>Employee ID</t>
+  </si>
+  <si>
+    <t>Amount</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,8 +239,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -415,8 +439,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF228B22"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -531,8 +561,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -576,16 +621,19 @@
     <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="10" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="44">
     <cellStyle name="20% - Accent1 2" xfId="20" xr:uid="{4FB1FAA9-738E-4B95-A8A9-57C1B30794A6}"/>
     <cellStyle name="20% - Accent2 2" xfId="24" xr:uid="{BC1D39A5-C7D9-444A-B41B-83D303D7AB09}"/>
     <cellStyle name="20% - Accent3 2" xfId="28" xr:uid="{EE161F90-D78E-441B-901D-A22BBB7DE7C3}"/>
@@ -624,6 +672,7 @@
     <cellStyle name="Neutral 2" xfId="9" xr:uid="{59F2A207-7A39-407A-8192-70C32E354A3F}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{142DF168-FBFF-45EF-AF4C-350649A1F72D}"/>
+    <cellStyle name="Normal 3" xfId="43" xr:uid="{6869CD9A-F29D-45E3-A20E-8B9DAF196893}"/>
     <cellStyle name="Note 2" xfId="16" xr:uid="{68C82225-C8FE-49CE-9C7E-5D1917AE3919}"/>
     <cellStyle name="Output 2" xfId="11" xr:uid="{611FA2F8-5D9D-49A5-AB46-4C4DFBECF35F}"/>
     <cellStyle name="Title 2" xfId="2" xr:uid="{D7A39A71-395B-484E-A80C-B4A9AE5D75E1}"/>
@@ -904,7 +953,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -926,58 +975,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
@@ -989,7 +1038,7 @@
         <v>45577</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I2">
         <v>2024</v>
@@ -997,13 +1046,13 @@
       <c r="J2" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="5">
+      <c r="K2" s="4">
         <v>111111</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L2" s="4">
         <v>0</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2" s="4">
         <v>111111</v>
       </c>
     </row>
@@ -1011,14 +1060,14 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
@@ -1030,7 +1079,7 @@
         <v>45577</v>
       </c>
       <c r="H3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I3">
         <v>2024</v>
@@ -1038,13 +1087,13 @@
       <c r="J3" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="4">
         <v>111111</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="4">
         <v>0</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="4">
         <v>111111</v>
       </c>
     </row>

</xml_diff>